<commit_message>
A 30-as maszk megoldvaxd
</commit_message>
<xml_diff>
--- a/ipcim.xlsx
+++ b/ipcim.xlsx
@@ -10,7 +10,7 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataSignature="AMtx7mhfXWjcZHZaIW73+VRz+M3FOT/UEw=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataSignature="AMtx7miJXMLNY6rUQ+YWnJC84EE+Ill/vw=="/>
     </ext>
   </extLst>
 </workbook>
@@ -310,7 +310,7 @@
     <t>10.0.0.1</t>
   </si>
   <si>
-    <t>255.0.0.0</t>
+    <t>255.255.255.252</t>
   </si>
   <si>
     <t>185.62.128.222</t>
@@ -390,7 +390,7 @@
     <numFmt numFmtId="164" formatCode="[$$]#,##0.00"/>
     <numFmt numFmtId="165" formatCode="#,##0.00\ [$Ft-40E]"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -432,6 +432,11 @@
       <sz val="24.0"/>
       <color theme="1"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <color rgb="FF000000"/>
+      <name val="Docs-Calibri"/>
     </font>
   </fonts>
   <fills count="11">
@@ -656,7 +661,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="55">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -716,6 +721,21 @@
     </xf>
     <xf borderId="1" fillId="2" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="1" fillId="10" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="4" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="5" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="6" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="7" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
     <xf borderId="11" fillId="10" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="14" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="15" fillId="0" fontId="6" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
@@ -6124,6 +6144,7 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
     <col customWidth="1" min="15" max="15" width="15.43"/>
+    <col customWidth="1" min="19" max="19" width="15.43"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -6240,7 +6261,7 @@
       <c r="R3" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="S3" s="11" t="s">
+      <c r="S3" s="37" t="s">
         <v>97</v>
       </c>
     </row>
@@ -6287,7 +6308,7 @@
       <c r="R4" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="S4" s="11" t="s">
+      <c r="S4" s="38" t="s">
         <v>97</v>
       </c>
     </row>
@@ -6392,7 +6413,7 @@
       <c r="R7" s="17" t="s">
         <v>102</v>
       </c>
-      <c r="S7" s="17" t="s">
+      <c r="S7" s="39" t="s">
         <v>97</v>
       </c>
     </row>
@@ -6437,7 +6458,7 @@
       <c r="R8" s="17" t="s">
         <v>103</v>
       </c>
-      <c r="S8" s="17" t="s">
+      <c r="S8" s="39" t="s">
         <v>97</v>
       </c>
     </row>
@@ -6569,7 +6590,7 @@
       <c r="R11" s="19" t="s">
         <v>108</v>
       </c>
-      <c r="S11" s="19" t="s">
+      <c r="S11" s="40" t="s">
         <v>97</v>
       </c>
     </row>
@@ -6607,7 +6628,7 @@
       <c r="R12" s="19" t="s">
         <v>109</v>
       </c>
-      <c r="S12" s="19" t="s">
+      <c r="S12" s="40" t="s">
         <v>97</v>
       </c>
     </row>
@@ -6712,7 +6733,7 @@
       <c r="R15" s="21" t="s">
         <v>111</v>
       </c>
-      <c r="S15" s="21" t="s">
+      <c r="S15" s="41" t="s">
         <v>97</v>
       </c>
     </row>
@@ -6750,7 +6771,7 @@
       <c r="R16" s="21" t="s">
         <v>113</v>
       </c>
-      <c r="S16" s="21" t="s">
+      <c r="S16" s="41" t="s">
         <v>97</v>
       </c>
     </row>
@@ -6811,7 +6832,7 @@
       <c r="K18" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="M18" s="37" t="s">
+      <c r="M18" s="42" t="s">
         <v>87</v>
       </c>
       <c r="N18" s="31"/>
@@ -6844,12 +6865,12 @@
         <v>209.0</v>
       </c>
       <c r="K19" s="27"/>
-      <c r="M19" s="38" t="s">
+      <c r="M19" s="43" t="s">
         <v>114</v>
       </c>
-      <c r="N19" s="39"/>
-      <c r="O19" s="39"/>
-      <c r="P19" s="40"/>
+      <c r="N19" s="44"/>
+      <c r="O19" s="44"/>
+      <c r="P19" s="45"/>
     </row>
     <row r="20">
       <c r="A20" s="3" t="s">
@@ -6877,13 +6898,13 @@
         <v>210.0</v>
       </c>
       <c r="K20" s="27"/>
-      <c r="M20" s="41">
+      <c r="M20" s="46">
         <v>185.0</v>
       </c>
-      <c r="N20" s="42">
+      <c r="N20" s="47">
         <v>62.0</v>
       </c>
-      <c r="O20" s="42">
+      <c r="O20" s="47">
         <v>128.0</v>
       </c>
       <c r="P20" s="13">
@@ -6916,15 +6937,15 @@
         <v>211.0</v>
       </c>
       <c r="K21" s="27"/>
-      <c r="M21" s="43" t="str">
+      <c r="M21" s="48" t="str">
         <f t="shared" ref="M21:P21" si="1">DEC2BIN(M20,8)</f>
         <v>10111001</v>
       </c>
-      <c r="N21" s="44" t="str">
+      <c r="N21" s="49" t="str">
         <f t="shared" si="1"/>
         <v>00111110</v>
       </c>
-      <c r="O21" s="44" t="str">
+      <c r="O21" s="49" t="str">
         <f t="shared" si="1"/>
         <v>10000000</v>
       </c>
@@ -6932,7 +6953,7 @@
         <f t="shared" si="1"/>
         <v>00000000</v>
       </c>
-      <c r="R21" s="45" t="s">
+      <c r="R21" s="50" t="s">
         <v>115</v>
       </c>
       <c r="S21" s="32"/>
@@ -6963,17 +6984,17 @@
         <v>212.0</v>
       </c>
       <c r="K22" s="27"/>
-      <c r="M22" s="38" t="s">
+      <c r="M22" s="43" t="s">
         <v>116</v>
       </c>
-      <c r="N22" s="39"/>
-      <c r="O22" s="39"/>
-      <c r="P22" s="40"/>
-      <c r="R22" s="46">
+      <c r="N22" s="44"/>
+      <c r="O22" s="44"/>
+      <c r="P22" s="45"/>
+      <c r="R22" s="51">
         <f>(127+63+31+16)*51</f>
         <v>12087</v>
       </c>
-      <c r="S22" s="47">
+      <c r="S22" s="52">
         <f>R22*394</f>
         <v>4762278</v>
       </c>
@@ -7004,22 +7025,22 @@
         <v>213.0</v>
       </c>
       <c r="K23" s="27"/>
-      <c r="M23" s="41">
+      <c r="M23" s="46">
         <v>185.0</v>
       </c>
-      <c r="N23" s="42">
+      <c r="N23" s="47">
         <v>62.0</v>
       </c>
-      <c r="O23" s="42">
+      <c r="O23" s="47">
         <v>128.0</v>
       </c>
       <c r="P23" s="13">
         <v>1.0</v>
       </c>
-      <c r="S23" s="42"/>
-      <c r="T23" s="42"/>
-      <c r="U23" s="42"/>
-      <c r="V23" s="42"/>
+      <c r="S23" s="47"/>
+      <c r="T23" s="47"/>
+      <c r="U23" s="47"/>
+      <c r="V23" s="47"/>
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="3" t="s">
@@ -7047,15 +7068,15 @@
         <v>214.0</v>
       </c>
       <c r="K24" s="27"/>
-      <c r="M24" s="43" t="str">
+      <c r="M24" s="48" t="str">
         <f t="shared" ref="M24:P24" si="2">DEC2BIN(M23,8)</f>
         <v>10111001</v>
       </c>
-      <c r="N24" s="44" t="str">
+      <c r="N24" s="49" t="str">
         <f t="shared" si="2"/>
         <v>00111110</v>
       </c>
-      <c r="O24" s="44" t="str">
+      <c r="O24" s="49" t="str">
         <f t="shared" si="2"/>
         <v>10000000</v>
       </c>
@@ -7063,10 +7084,10 @@
         <f t="shared" si="2"/>
         <v>00000001</v>
       </c>
-      <c r="S24" s="42"/>
-      <c r="T24" s="42"/>
-      <c r="U24" s="42"/>
-      <c r="V24" s="42"/>
+      <c r="S24" s="47"/>
+      <c r="T24" s="47"/>
+      <c r="U24" s="47"/>
+      <c r="V24" s="47"/>
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="3" t="s">
@@ -7094,16 +7115,16 @@
         <v>215.0</v>
       </c>
       <c r="K25" s="27"/>
-      <c r="M25" s="38" t="s">
+      <c r="M25" s="43" t="s">
         <v>117</v>
       </c>
-      <c r="N25" s="39"/>
-      <c r="O25" s="39"/>
-      <c r="P25" s="40"/>
-      <c r="S25" s="42"/>
-      <c r="T25" s="42"/>
-      <c r="U25" s="42"/>
-      <c r="V25" s="42"/>
+      <c r="N25" s="44"/>
+      <c r="O25" s="44"/>
+      <c r="P25" s="45"/>
+      <c r="S25" s="47"/>
+      <c r="T25" s="47"/>
+      <c r="U25" s="47"/>
+      <c r="V25" s="47"/>
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="3" t="s">
@@ -7131,22 +7152,22 @@
         <v>216.0</v>
       </c>
       <c r="K26" s="27"/>
-      <c r="M26" s="41">
+      <c r="M26" s="46">
         <v>185.0</v>
       </c>
-      <c r="N26" s="42">
+      <c r="N26" s="47">
         <v>62.0</v>
       </c>
-      <c r="O26" s="42">
+      <c r="O26" s="47">
         <v>128.0</v>
       </c>
       <c r="P26" s="13">
         <v>2.0</v>
       </c>
-      <c r="S26" s="42"/>
-      <c r="T26" s="42"/>
-      <c r="U26" s="42"/>
-      <c r="V26" s="42"/>
+      <c r="S26" s="47"/>
+      <c r="T26" s="47"/>
+      <c r="U26" s="47"/>
+      <c r="V26" s="47"/>
     </row>
     <row r="27" ht="15.75" customHeight="1">
       <c r="A27" s="3" t="s">
@@ -7174,15 +7195,15 @@
         <v>217.0</v>
       </c>
       <c r="K27" s="27"/>
-      <c r="M27" s="43" t="str">
+      <c r="M27" s="48" t="str">
         <f t="shared" ref="M27:P27" si="3">DEC2BIN(M26,8)</f>
         <v>10111001</v>
       </c>
-      <c r="N27" s="44" t="str">
+      <c r="N27" s="49" t="str">
         <f t="shared" si="3"/>
         <v>00111110</v>
       </c>
-      <c r="O27" s="44" t="str">
+      <c r="O27" s="49" t="str">
         <f t="shared" si="3"/>
         <v>10000000</v>
       </c>
@@ -7190,10 +7211,10 @@
         <f t="shared" si="3"/>
         <v>00000010</v>
       </c>
-      <c r="S27" s="42"/>
-      <c r="T27" s="42"/>
-      <c r="U27" s="42"/>
-      <c r="V27" s="42"/>
+      <c r="S27" s="47"/>
+      <c r="T27" s="47"/>
+      <c r="U27" s="47"/>
+      <c r="V27" s="47"/>
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="A28" s="3" t="s">
@@ -7221,16 +7242,16 @@
         <v>218.0</v>
       </c>
       <c r="K28" s="27"/>
-      <c r="M28" s="38" t="s">
+      <c r="M28" s="43" t="s">
         <v>118</v>
       </c>
-      <c r="N28" s="39"/>
-      <c r="O28" s="39"/>
-      <c r="P28" s="40"/>
-      <c r="S28" s="42"/>
-      <c r="T28" s="42"/>
-      <c r="U28" s="42"/>
-      <c r="V28" s="42"/>
+      <c r="N28" s="44"/>
+      <c r="O28" s="44"/>
+      <c r="P28" s="45"/>
+      <c r="S28" s="47"/>
+      <c r="T28" s="47"/>
+      <c r="U28" s="47"/>
+      <c r="V28" s="47"/>
     </row>
     <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="3" t="s">
@@ -7258,22 +7279,22 @@
         <v>219.0</v>
       </c>
       <c r="K29" s="27"/>
-      <c r="M29" s="41">
+      <c r="M29" s="46">
         <v>185.0</v>
       </c>
-      <c r="N29" s="42">
+      <c r="N29" s="47">
         <v>62.0</v>
       </c>
-      <c r="O29" s="42">
+      <c r="O29" s="47">
         <v>128.0</v>
       </c>
       <c r="P29" s="13">
         <v>126.0</v>
       </c>
-      <c r="S29" s="42"/>
-      <c r="T29" s="42"/>
-      <c r="U29" s="42"/>
-      <c r="V29" s="42"/>
+      <c r="S29" s="47"/>
+      <c r="T29" s="47"/>
+      <c r="U29" s="47"/>
+      <c r="V29" s="47"/>
     </row>
     <row r="30" ht="15.75" customHeight="1">
       <c r="A30" s="3" t="s">
@@ -7301,15 +7322,15 @@
         <v>220.0</v>
       </c>
       <c r="K30" s="27"/>
-      <c r="M30" s="43" t="str">
+      <c r="M30" s="48" t="str">
         <f t="shared" ref="M30:P30" si="4">DEC2BIN(M29,8)</f>
         <v>10111001</v>
       </c>
-      <c r="N30" s="44" t="str">
+      <c r="N30" s="49" t="str">
         <f t="shared" si="4"/>
         <v>00111110</v>
       </c>
-      <c r="O30" s="44" t="str">
+      <c r="O30" s="49" t="str">
         <f t="shared" si="4"/>
         <v>10000000</v>
       </c>
@@ -7317,10 +7338,10 @@
         <f t="shared" si="4"/>
         <v>01111110</v>
       </c>
-      <c r="S30" s="42"/>
-      <c r="T30" s="42"/>
-      <c r="U30" s="42"/>
-      <c r="V30" s="42"/>
+      <c r="S30" s="47"/>
+      <c r="T30" s="47"/>
+      <c r="U30" s="47"/>
+      <c r="V30" s="47"/>
     </row>
     <row r="31" ht="15.75" customHeight="1">
       <c r="A31" s="3" t="s">
@@ -7348,17 +7369,17 @@
         <v>221.0</v>
       </c>
       <c r="K31" s="27"/>
-      <c r="M31" s="38" t="s">
+      <c r="M31" s="43" t="s">
         <v>119</v>
       </c>
-      <c r="N31" s="39"/>
-      <c r="O31" s="39"/>
-      <c r="P31" s="40"/>
-      <c r="R31" s="42"/>
-      <c r="S31" s="42"/>
-      <c r="T31" s="42"/>
-      <c r="U31" s="42"/>
-      <c r="V31" s="42"/>
+      <c r="N31" s="44"/>
+      <c r="O31" s="44"/>
+      <c r="P31" s="45"/>
+      <c r="R31" s="47"/>
+      <c r="S31" s="47"/>
+      <c r="T31" s="47"/>
+      <c r="U31" s="47"/>
+      <c r="V31" s="47"/>
     </row>
     <row r="32" ht="15.75" customHeight="1">
       <c r="A32" s="3" t="s">
@@ -7388,23 +7409,23 @@
       <c r="K32" s="27" t="s">
         <v>86</v>
       </c>
-      <c r="M32" s="41">
+      <c r="M32" s="46">
         <v>185.0</v>
       </c>
-      <c r="N32" s="42">
+      <c r="N32" s="47">
         <v>62.0</v>
       </c>
-      <c r="O32" s="42">
+      <c r="O32" s="47">
         <v>128.0</v>
       </c>
       <c r="P32" s="13">
         <v>127.0</v>
       </c>
-      <c r="R32" s="42"/>
-      <c r="S32" s="42"/>
-      <c r="T32" s="42"/>
-      <c r="U32" s="42"/>
-      <c r="V32" s="42"/>
+      <c r="R32" s="47"/>
+      <c r="S32" s="47"/>
+      <c r="T32" s="47"/>
+      <c r="U32" s="47"/>
+      <c r="V32" s="47"/>
     </row>
     <row r="33" ht="15.75" customHeight="1">
       <c r="A33" s="3" t="s">
@@ -7434,15 +7455,15 @@
       <c r="K33" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="M33" s="43" t="str">
+      <c r="M33" s="48" t="str">
         <f t="shared" ref="M33:P33" si="5">DEC2BIN(M32,8)</f>
         <v>10111001</v>
       </c>
-      <c r="N33" s="44" t="str">
+      <c r="N33" s="49" t="str">
         <f t="shared" si="5"/>
         <v>00111110</v>
       </c>
-      <c r="O33" s="44" t="str">
+      <c r="O33" s="49" t="str">
         <f t="shared" si="5"/>
         <v>10000000</v>
       </c>
@@ -7450,11 +7471,11 @@
         <f t="shared" si="5"/>
         <v>01111111</v>
       </c>
-      <c r="R33" s="42"/>
-      <c r="S33" s="42"/>
-      <c r="T33" s="42"/>
-      <c r="U33" s="42"/>
-      <c r="V33" s="42"/>
+      <c r="R33" s="47"/>
+      <c r="S33" s="47"/>
+      <c r="T33" s="47"/>
+      <c r="U33" s="47"/>
+      <c r="V33" s="47"/>
     </row>
     <row r="34" ht="15.75" customHeight="1">
       <c r="A34" s="3" t="s">
@@ -7473,19 +7494,19 @@
         <v>160.0</v>
       </c>
       <c r="G34" s="25"/>
-      <c r="M34" s="38" t="s">
+      <c r="M34" s="43" t="s">
         <v>120</v>
       </c>
-      <c r="N34" s="39"/>
-      <c r="O34" s="39"/>
+      <c r="N34" s="44"/>
+      <c r="O34" s="44"/>
       <c r="P34" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="R34" s="42"/>
-      <c r="S34" s="42"/>
-      <c r="T34" s="42"/>
-      <c r="U34" s="42"/>
-      <c r="V34" s="42"/>
+      <c r="R34" s="47"/>
+      <c r="S34" s="47"/>
+      <c r="T34" s="47"/>
+      <c r="U34" s="47"/>
+      <c r="V34" s="47"/>
     </row>
     <row r="35" ht="15.75" customHeight="1">
       <c r="A35" s="3" t="s">
@@ -7504,23 +7525,23 @@
         <v>161.0</v>
       </c>
       <c r="G35" s="25"/>
-      <c r="M35" s="41">
+      <c r="M35" s="46">
         <v>255.0</v>
       </c>
-      <c r="N35" s="42">
+      <c r="N35" s="47">
         <v>255.0</v>
       </c>
-      <c r="O35" s="42">
+      <c r="O35" s="47">
         <v>255.0</v>
       </c>
       <c r="P35" s="13">
         <v>128.0</v>
       </c>
-      <c r="R35" s="42"/>
-      <c r="S35" s="42"/>
-      <c r="T35" s="42"/>
-      <c r="U35" s="42"/>
-      <c r="V35" s="42"/>
+      <c r="R35" s="47"/>
+      <c r="S35" s="47"/>
+      <c r="T35" s="47"/>
+      <c r="U35" s="47"/>
+      <c r="V35" s="47"/>
     </row>
     <row r="36" ht="15.75" customHeight="1">
       <c r="A36" s="3" t="s">
@@ -7548,15 +7569,15 @@
       <c r="K36" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="M36" s="43" t="str">
+      <c r="M36" s="48" t="str">
         <f t="shared" ref="M36:P36" si="6">DEC2BIN(M35,8)</f>
         <v>11111111</v>
       </c>
-      <c r="N36" s="44" t="str">
+      <c r="N36" s="49" t="str">
         <f t="shared" si="6"/>
         <v>11111111</v>
       </c>
-      <c r="O36" s="44" t="str">
+      <c r="O36" s="49" t="str">
         <f t="shared" si="6"/>
         <v>11111111</v>
       </c>
@@ -7564,11 +7585,11 @@
         <f t="shared" si="6"/>
         <v>10000000</v>
       </c>
-      <c r="R36" s="42"/>
-      <c r="S36" s="42"/>
-      <c r="T36" s="42"/>
-      <c r="U36" s="42"/>
-      <c r="V36" s="42"/>
+      <c r="R36" s="47"/>
+      <c r="S36" s="47"/>
+      <c r="T36" s="47"/>
+      <c r="U36" s="47"/>
+      <c r="V36" s="47"/>
     </row>
     <row r="37" ht="15.75" customHeight="1">
       <c r="A37" s="3" t="s">
@@ -7596,14 +7617,14 @@
       <c r="K37" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="M37" s="42"/>
-      <c r="N37" s="42"/>
-      <c r="O37" s="42"/>
-      <c r="P37" s="42"/>
-      <c r="S37" s="42"/>
-      <c r="T37" s="42"/>
-      <c r="U37" s="42"/>
-      <c r="V37" s="42"/>
+      <c r="M37" s="47"/>
+      <c r="N37" s="47"/>
+      <c r="O37" s="47"/>
+      <c r="P37" s="47"/>
+      <c r="S37" s="47"/>
+      <c r="T37" s="47"/>
+      <c r="U37" s="47"/>
+      <c r="V37" s="47"/>
     </row>
     <row r="38" ht="15.75" customHeight="1">
       <c r="A38" s="3" t="s">
@@ -7631,16 +7652,16 @@
       <c r="K38" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="M38" s="48" t="s">
+      <c r="M38" s="53" t="s">
         <v>88</v>
       </c>
       <c r="N38" s="31"/>
       <c r="O38" s="31"/>
       <c r="P38" s="32"/>
-      <c r="S38" s="42"/>
-      <c r="T38" s="42"/>
-      <c r="U38" s="42"/>
-      <c r="V38" s="42"/>
+      <c r="S38" s="47"/>
+      <c r="T38" s="47"/>
+      <c r="U38" s="47"/>
+      <c r="V38" s="47"/>
     </row>
     <row r="39" ht="15.75" customHeight="1">
       <c r="A39" s="3" t="s">
@@ -7668,16 +7689,16 @@
       <c r="K39" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="M39" s="38" t="s">
+      <c r="M39" s="43" t="s">
         <v>114</v>
       </c>
-      <c r="N39" s="39"/>
-      <c r="O39" s="39"/>
-      <c r="P39" s="40"/>
-      <c r="S39" s="42"/>
-      <c r="T39" s="42"/>
-      <c r="U39" s="42"/>
-      <c r="V39" s="42"/>
+      <c r="N39" s="44"/>
+      <c r="O39" s="44"/>
+      <c r="P39" s="45"/>
+      <c r="S39" s="47"/>
+      <c r="T39" s="47"/>
+      <c r="U39" s="47"/>
+      <c r="V39" s="47"/>
     </row>
     <row r="40" ht="15.75" customHeight="1">
       <c r="A40" s="3" t="s">
@@ -7705,22 +7726,22 @@
       <c r="K40" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="M40" s="41">
+      <c r="M40" s="46">
         <v>185.0</v>
       </c>
-      <c r="N40" s="42">
+      <c r="N40" s="47">
         <v>62.0</v>
       </c>
-      <c r="O40" s="42">
+      <c r="O40" s="47">
         <v>128.0</v>
       </c>
       <c r="P40" s="13">
         <v>128.0</v>
       </c>
-      <c r="S40" s="42"/>
-      <c r="T40" s="42"/>
-      <c r="U40" s="42"/>
-      <c r="V40" s="42"/>
+      <c r="S40" s="47"/>
+      <c r="T40" s="47"/>
+      <c r="U40" s="47"/>
+      <c r="V40" s="47"/>
     </row>
     <row r="41" ht="15.75" customHeight="1">
       <c r="A41" s="3" t="s">
@@ -7748,15 +7769,15 @@
       <c r="K41" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="M41" s="43" t="str">
+      <c r="M41" s="48" t="str">
         <f t="shared" ref="M41:P41" si="7">DEC2BIN(M40,8)</f>
         <v>10111001</v>
       </c>
-      <c r="N41" s="44" t="str">
+      <c r="N41" s="49" t="str">
         <f t="shared" si="7"/>
         <v>00111110</v>
       </c>
-      <c r="O41" s="44" t="str">
+      <c r="O41" s="49" t="str">
         <f t="shared" si="7"/>
         <v>10000000</v>
       </c>
@@ -7764,10 +7785,10 @@
         <f t="shared" si="7"/>
         <v>10000000</v>
       </c>
-      <c r="S41" s="42"/>
-      <c r="T41" s="42"/>
-      <c r="U41" s="42"/>
-      <c r="V41" s="42"/>
+      <c r="S41" s="47"/>
+      <c r="T41" s="47"/>
+      <c r="U41" s="47"/>
+      <c r="V41" s="47"/>
     </row>
     <row r="42" ht="15.75" customHeight="1">
       <c r="A42" s="3" t="s">
@@ -7795,16 +7816,16 @@
       <c r="K42" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="M42" s="38" t="s">
+      <c r="M42" s="43" t="s">
         <v>116</v>
       </c>
-      <c r="N42" s="39"/>
-      <c r="O42" s="39"/>
-      <c r="P42" s="40"/>
-      <c r="S42" s="42"/>
-      <c r="T42" s="42"/>
-      <c r="U42" s="42"/>
-      <c r="V42" s="42"/>
+      <c r="N42" s="44"/>
+      <c r="O42" s="44"/>
+      <c r="P42" s="45"/>
+      <c r="S42" s="47"/>
+      <c r="T42" s="47"/>
+      <c r="U42" s="47"/>
+      <c r="V42" s="47"/>
     </row>
     <row r="43" ht="15.75" customHeight="1">
       <c r="A43" s="3" t="s">
@@ -7832,22 +7853,22 @@
       <c r="K43" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="M43" s="41">
+      <c r="M43" s="46">
         <v>185.0</v>
       </c>
-      <c r="N43" s="42">
+      <c r="N43" s="47">
         <v>62.0</v>
       </c>
-      <c r="O43" s="42">
+      <c r="O43" s="47">
         <v>128.0</v>
       </c>
       <c r="P43" s="13">
         <v>129.0</v>
       </c>
-      <c r="S43" s="42"/>
-      <c r="T43" s="42"/>
-      <c r="U43" s="42"/>
-      <c r="V43" s="42"/>
+      <c r="S43" s="47"/>
+      <c r="T43" s="47"/>
+      <c r="U43" s="47"/>
+      <c r="V43" s="47"/>
     </row>
     <row r="44" ht="15.75" customHeight="1">
       <c r="A44" s="3" t="s">
@@ -7875,15 +7896,15 @@
       <c r="K44" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="M44" s="43" t="str">
+      <c r="M44" s="48" t="str">
         <f t="shared" ref="M44:P44" si="8">DEC2BIN(M43,8)</f>
         <v>10111001</v>
       </c>
-      <c r="N44" s="44" t="str">
+      <c r="N44" s="49" t="str">
         <f t="shared" si="8"/>
         <v>00111110</v>
       </c>
-      <c r="O44" s="44" t="str">
+      <c r="O44" s="49" t="str">
         <f t="shared" si="8"/>
         <v>10000000</v>
       </c>
@@ -7891,10 +7912,10 @@
         <f t="shared" si="8"/>
         <v>10000001</v>
       </c>
-      <c r="S44" s="42"/>
-      <c r="T44" s="42"/>
-      <c r="U44" s="42"/>
-      <c r="V44" s="42"/>
+      <c r="S44" s="47"/>
+      <c r="T44" s="47"/>
+      <c r="U44" s="47"/>
+      <c r="V44" s="47"/>
     </row>
     <row r="45" ht="15.75" customHeight="1">
       <c r="A45" s="3" t="s">
@@ -7922,16 +7943,16 @@
       <c r="K45" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="M45" s="38" t="s">
+      <c r="M45" s="43" t="s">
         <v>117</v>
       </c>
-      <c r="N45" s="39"/>
-      <c r="O45" s="39"/>
-      <c r="P45" s="40"/>
-      <c r="S45" s="42"/>
-      <c r="T45" s="42"/>
-      <c r="U45" s="42"/>
-      <c r="V45" s="42"/>
+      <c r="N45" s="44"/>
+      <c r="O45" s="44"/>
+      <c r="P45" s="45"/>
+      <c r="S45" s="47"/>
+      <c r="T45" s="47"/>
+      <c r="U45" s="47"/>
+      <c r="V45" s="47"/>
     </row>
     <row r="46" ht="15.75" customHeight="1">
       <c r="A46" s="3" t="s">
@@ -7959,22 +7980,22 @@
       <c r="K46" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="M46" s="41">
+      <c r="M46" s="46">
         <v>185.0</v>
       </c>
-      <c r="N46" s="42">
+      <c r="N46" s="47">
         <v>62.0</v>
       </c>
-      <c r="O46" s="42">
+      <c r="O46" s="47">
         <v>128.0</v>
       </c>
       <c r="P46" s="13">
         <v>130.0</v>
       </c>
-      <c r="S46" s="42"/>
-      <c r="T46" s="42"/>
-      <c r="U46" s="42"/>
-      <c r="V46" s="42"/>
+      <c r="S46" s="47"/>
+      <c r="T46" s="47"/>
+      <c r="U46" s="47"/>
+      <c r="V46" s="47"/>
     </row>
     <row r="47" ht="15.75" customHeight="1">
       <c r="A47" s="3" t="s">
@@ -8002,15 +8023,15 @@
       <c r="K47" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="M47" s="43" t="str">
+      <c r="M47" s="48" t="str">
         <f t="shared" ref="M47:P47" si="9">DEC2BIN(M46,8)</f>
         <v>10111001</v>
       </c>
-      <c r="N47" s="44" t="str">
+      <c r="N47" s="49" t="str">
         <f t="shared" si="9"/>
         <v>00111110</v>
       </c>
-      <c r="O47" s="44" t="str">
+      <c r="O47" s="49" t="str">
         <f t="shared" si="9"/>
         <v>10000000</v>
       </c>
@@ -8018,10 +8039,10 @@
         <f t="shared" si="9"/>
         <v>10000010</v>
       </c>
-      <c r="S47" s="42"/>
-      <c r="T47" s="42"/>
-      <c r="U47" s="42"/>
-      <c r="V47" s="42"/>
+      <c r="S47" s="47"/>
+      <c r="T47" s="47"/>
+      <c r="U47" s="47"/>
+      <c r="V47" s="47"/>
     </row>
     <row r="48" ht="15.75" customHeight="1">
       <c r="A48" s="3" t="s">
@@ -8049,16 +8070,16 @@
       <c r="K48" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="M48" s="38" t="s">
+      <c r="M48" s="43" t="s">
         <v>118</v>
       </c>
-      <c r="N48" s="39"/>
-      <c r="O48" s="39"/>
-      <c r="P48" s="40"/>
-      <c r="S48" s="42"/>
-      <c r="T48" s="42"/>
-      <c r="U48" s="42"/>
-      <c r="V48" s="42"/>
+      <c r="N48" s="44"/>
+      <c r="O48" s="44"/>
+      <c r="P48" s="45"/>
+      <c r="S48" s="47"/>
+      <c r="T48" s="47"/>
+      <c r="U48" s="47"/>
+      <c r="V48" s="47"/>
     </row>
     <row r="49" ht="15.75" customHeight="1">
       <c r="A49" s="3" t="s">
@@ -8086,22 +8107,22 @@
       <c r="K49" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="M49" s="41">
+      <c r="M49" s="46">
         <v>185.0</v>
       </c>
-      <c r="N49" s="42">
+      <c r="N49" s="47">
         <v>62.0</v>
       </c>
-      <c r="O49" s="42">
+      <c r="O49" s="47">
         <v>128.0</v>
       </c>
       <c r="P49" s="13">
         <v>190.0</v>
       </c>
-      <c r="S49" s="42"/>
-      <c r="T49" s="42"/>
-      <c r="U49" s="42"/>
-      <c r="V49" s="42"/>
+      <c r="S49" s="47"/>
+      <c r="T49" s="47"/>
+      <c r="U49" s="47"/>
+      <c r="V49" s="47"/>
     </row>
     <row r="50" ht="15.75" customHeight="1">
       <c r="A50" s="3" t="s">
@@ -8129,15 +8150,15 @@
       <c r="K50" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="M50" s="43" t="str">
+      <c r="M50" s="48" t="str">
         <f t="shared" ref="M50:P50" si="10">DEC2BIN(M49,8)</f>
         <v>10111001</v>
       </c>
-      <c r="N50" s="44" t="str">
+      <c r="N50" s="49" t="str">
         <f t="shared" si="10"/>
         <v>00111110</v>
       </c>
-      <c r="O50" s="44" t="str">
+      <c r="O50" s="49" t="str">
         <f t="shared" si="10"/>
         <v>10000000</v>
       </c>
@@ -8145,10 +8166,10 @@
         <f t="shared" si="10"/>
         <v>10111110</v>
       </c>
-      <c r="S50" s="42"/>
-      <c r="T50" s="42"/>
-      <c r="U50" s="42"/>
-      <c r="V50" s="42"/>
+      <c r="S50" s="47"/>
+      <c r="T50" s="47"/>
+      <c r="U50" s="47"/>
+      <c r="V50" s="47"/>
     </row>
     <row r="51" ht="15.75" customHeight="1">
       <c r="A51" s="3" t="s">
@@ -8176,16 +8197,16 @@
       <c r="K51" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="M51" s="38" t="s">
+      <c r="M51" s="43" t="s">
         <v>119</v>
       </c>
-      <c r="N51" s="39"/>
-      <c r="O51" s="39"/>
-      <c r="P51" s="40"/>
-      <c r="S51" s="42"/>
-      <c r="T51" s="42"/>
-      <c r="U51" s="42"/>
-      <c r="V51" s="42"/>
+      <c r="N51" s="44"/>
+      <c r="O51" s="44"/>
+      <c r="P51" s="45"/>
+      <c r="S51" s="47"/>
+      <c r="T51" s="47"/>
+      <c r="U51" s="47"/>
+      <c r="V51" s="47"/>
     </row>
     <row r="52" ht="15.75" customHeight="1">
       <c r="A52" s="3" t="s">
@@ -8204,22 +8225,22 @@
         <v>178.0</v>
       </c>
       <c r="G52" s="25"/>
-      <c r="M52" s="41">
+      <c r="M52" s="46">
         <v>185.0</v>
       </c>
-      <c r="N52" s="42">
+      <c r="N52" s="47">
         <v>62.0</v>
       </c>
-      <c r="O52" s="42">
+      <c r="O52" s="47">
         <v>128.0</v>
       </c>
       <c r="P52" s="13">
         <v>191.0</v>
       </c>
-      <c r="S52" s="42"/>
-      <c r="T52" s="42"/>
-      <c r="U52" s="42"/>
-      <c r="V52" s="42"/>
+      <c r="S52" s="47"/>
+      <c r="T52" s="47"/>
+      <c r="U52" s="47"/>
+      <c r="V52" s="47"/>
     </row>
     <row r="53" ht="15.75" customHeight="1">
       <c r="A53" s="3" t="s">
@@ -8238,15 +8259,15 @@
         <v>179.0</v>
       </c>
       <c r="G53" s="25"/>
-      <c r="M53" s="43" t="str">
+      <c r="M53" s="48" t="str">
         <f t="shared" ref="M53:P53" si="11">DEC2BIN(M52,8)</f>
         <v>10111001</v>
       </c>
-      <c r="N53" s="44" t="str">
+      <c r="N53" s="49" t="str">
         <f t="shared" si="11"/>
         <v>00111110</v>
       </c>
-      <c r="O53" s="44" t="str">
+      <c r="O53" s="49" t="str">
         <f t="shared" si="11"/>
         <v>10000000</v>
       </c>
@@ -8272,11 +8293,11 @@
         <v>180.0</v>
       </c>
       <c r="G54" s="25"/>
-      <c r="M54" s="38" t="s">
+      <c r="M54" s="43" t="s">
         <v>120</v>
       </c>
-      <c r="N54" s="39"/>
-      <c r="O54" s="39"/>
+      <c r="N54" s="44"/>
+      <c r="O54" s="44"/>
       <c r="P54" s="13" t="s">
         <v>4</v>
       </c>
@@ -8298,13 +8319,13 @@
         <v>181.0</v>
       </c>
       <c r="G55" s="25"/>
-      <c r="M55" s="41">
+      <c r="M55" s="46">
         <v>255.0</v>
       </c>
-      <c r="N55" s="42">
+      <c r="N55" s="47">
         <v>255.0</v>
       </c>
-      <c r="O55" s="42">
+      <c r="O55" s="47">
         <v>255.0</v>
       </c>
       <c r="P55" s="13">
@@ -8328,15 +8349,15 @@
         <v>182.0</v>
       </c>
       <c r="G56" s="25"/>
-      <c r="M56" s="43" t="str">
+      <c r="M56" s="48" t="str">
         <f t="shared" ref="M56:P56" si="12">DEC2BIN(M55,8)</f>
         <v>11111111</v>
       </c>
-      <c r="N56" s="44" t="str">
+      <c r="N56" s="49" t="str">
         <f t="shared" si="12"/>
         <v>11111111</v>
       </c>
-      <c r="O56" s="44" t="str">
+      <c r="O56" s="49" t="str">
         <f t="shared" si="12"/>
         <v>11111111</v>
       </c>
@@ -8362,10 +8383,10 @@
         <v>183.0</v>
       </c>
       <c r="G57" s="25"/>
-      <c r="M57" s="42"/>
-      <c r="N57" s="42"/>
-      <c r="O57" s="42"/>
-      <c r="P57" s="42"/>
+      <c r="M57" s="47"/>
+      <c r="N57" s="47"/>
+      <c r="O57" s="47"/>
+      <c r="P57" s="47"/>
     </row>
     <row r="58" ht="15.75" customHeight="1">
       <c r="A58" s="3" t="s">
@@ -8384,7 +8405,7 @@
         <v>184.0</v>
       </c>
       <c r="G58" s="25"/>
-      <c r="M58" s="49" t="s">
+      <c r="M58" s="54" t="s">
         <v>89</v>
       </c>
       <c r="N58" s="31"/>
@@ -8408,12 +8429,12 @@
         <v>185.0</v>
       </c>
       <c r="G59" s="25"/>
-      <c r="M59" s="38" t="s">
+      <c r="M59" s="43" t="s">
         <v>114</v>
       </c>
-      <c r="N59" s="39"/>
-      <c r="O59" s="39"/>
-      <c r="P59" s="40"/>
+      <c r="N59" s="44"/>
+      <c r="O59" s="44"/>
+      <c r="P59" s="45"/>
     </row>
     <row r="60" ht="15.75" customHeight="1">
       <c r="A60" s="3" t="s">
@@ -8432,13 +8453,13 @@
         <v>186.0</v>
       </c>
       <c r="G60" s="25"/>
-      <c r="M60" s="41">
+      <c r="M60" s="46">
         <v>185.0</v>
       </c>
-      <c r="N60" s="42">
+      <c r="N60" s="47">
         <v>62.0</v>
       </c>
-      <c r="O60" s="42">
+      <c r="O60" s="47">
         <v>128.0</v>
       </c>
       <c r="P60" s="13">
@@ -8462,15 +8483,15 @@
         <v>187.0</v>
       </c>
       <c r="G61" s="25"/>
-      <c r="M61" s="43" t="str">
+      <c r="M61" s="48" t="str">
         <f t="shared" ref="M61:P61" si="13">DEC2BIN(M60,8)</f>
         <v>10111001</v>
       </c>
-      <c r="N61" s="44" t="str">
+      <c r="N61" s="49" t="str">
         <f t="shared" si="13"/>
         <v>00111110</v>
       </c>
-      <c r="O61" s="44" t="str">
+      <c r="O61" s="49" t="str">
         <f t="shared" si="13"/>
         <v>10000000</v>
       </c>
@@ -8496,12 +8517,12 @@
         <v>188.0</v>
       </c>
       <c r="G62" s="25"/>
-      <c r="M62" s="38" t="s">
+      <c r="M62" s="43" t="s">
         <v>116</v>
       </c>
-      <c r="N62" s="39"/>
-      <c r="O62" s="39"/>
-      <c r="P62" s="40"/>
+      <c r="N62" s="44"/>
+      <c r="O62" s="44"/>
+      <c r="P62" s="45"/>
     </row>
     <row r="63" ht="15.75" customHeight="1">
       <c r="A63" s="3" t="s">
@@ -8520,13 +8541,13 @@
         <v>189.0</v>
       </c>
       <c r="G63" s="25"/>
-      <c r="M63" s="41">
+      <c r="M63" s="46">
         <v>185.0</v>
       </c>
-      <c r="N63" s="42">
+      <c r="N63" s="47">
         <v>62.0</v>
       </c>
-      <c r="O63" s="42">
+      <c r="O63" s="47">
         <v>128.0</v>
       </c>
       <c r="P63" s="13">
@@ -8552,15 +8573,15 @@
       <c r="G64" s="25" t="s">
         <v>83</v>
       </c>
-      <c r="M64" s="43" t="str">
+      <c r="M64" s="48" t="str">
         <f t="shared" ref="M64:P64" si="14">DEC2BIN(M63,8)</f>
         <v>10111001</v>
       </c>
-      <c r="N64" s="44" t="str">
+      <c r="N64" s="49" t="str">
         <f t="shared" si="14"/>
         <v>00111110</v>
       </c>
-      <c r="O64" s="44" t="str">
+      <c r="O64" s="49" t="str">
         <f t="shared" si="14"/>
         <v>10000000</v>
       </c>
@@ -8586,12 +8607,12 @@
       <c r="G65" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="M65" s="38" t="s">
+      <c r="M65" s="43" t="s">
         <v>117</v>
       </c>
-      <c r="N65" s="39"/>
-      <c r="O65" s="39"/>
-      <c r="P65" s="40"/>
+      <c r="N65" s="44"/>
+      <c r="O65" s="44"/>
+      <c r="P65" s="45"/>
     </row>
     <row r="66" ht="15.75" customHeight="1">
       <c r="A66" s="3" t="s">
@@ -8601,13 +8622,13 @@
         <v>64.0</v>
       </c>
       <c r="C66" s="9"/>
-      <c r="M66" s="41">
+      <c r="M66" s="46">
         <v>185.0</v>
       </c>
-      <c r="N66" s="42">
+      <c r="N66" s="47">
         <v>62.0</v>
       </c>
-      <c r="O66" s="42">
+      <c r="O66" s="47">
         <v>128.0</v>
       </c>
       <c r="P66" s="13">
@@ -8622,15 +8643,15 @@
         <v>65.0</v>
       </c>
       <c r="C67" s="9"/>
-      <c r="M67" s="43" t="str">
+      <c r="M67" s="48" t="str">
         <f t="shared" ref="M67:P67" si="15">DEC2BIN(M66,8)</f>
         <v>10111001</v>
       </c>
-      <c r="N67" s="44" t="str">
+      <c r="N67" s="49" t="str">
         <f t="shared" si="15"/>
         <v>00111110</v>
       </c>
-      <c r="O67" s="44" t="str">
+      <c r="O67" s="49" t="str">
         <f t="shared" si="15"/>
         <v>10000000</v>
       </c>
@@ -8647,12 +8668,12 @@
         <v>66.0</v>
       </c>
       <c r="C68" s="9"/>
-      <c r="M68" s="38" t="s">
+      <c r="M68" s="43" t="s">
         <v>118</v>
       </c>
-      <c r="N68" s="39"/>
-      <c r="O68" s="39"/>
-      <c r="P68" s="40"/>
+      <c r="N68" s="44"/>
+      <c r="O68" s="44"/>
+      <c r="P68" s="45"/>
     </row>
     <row r="69" ht="15.75" customHeight="1">
       <c r="A69" s="3" t="s">
@@ -8662,13 +8683,13 @@
         <v>67.0</v>
       </c>
       <c r="C69" s="9"/>
-      <c r="M69" s="41">
+      <c r="M69" s="46">
         <v>185.0</v>
       </c>
-      <c r="N69" s="42">
+      <c r="N69" s="47">
         <v>62.0</v>
       </c>
-      <c r="O69" s="42">
+      <c r="O69" s="47">
         <v>128.0</v>
       </c>
       <c r="P69" s="13">
@@ -8683,15 +8704,15 @@
         <v>68.0</v>
       </c>
       <c r="C70" s="9"/>
-      <c r="M70" s="43" t="str">
+      <c r="M70" s="48" t="str">
         <f t="shared" ref="M70:P70" si="16">DEC2BIN(M69,8)</f>
         <v>10111001</v>
       </c>
-      <c r="N70" s="44" t="str">
+      <c r="N70" s="49" t="str">
         <f t="shared" si="16"/>
         <v>00111110</v>
       </c>
-      <c r="O70" s="44" t="str">
+      <c r="O70" s="49" t="str">
         <f t="shared" si="16"/>
         <v>10000000</v>
       </c>
@@ -8708,12 +8729,12 @@
         <v>69.0</v>
       </c>
       <c r="C71" s="9"/>
-      <c r="M71" s="38" t="s">
+      <c r="M71" s="43" t="s">
         <v>119</v>
       </c>
-      <c r="N71" s="39"/>
-      <c r="O71" s="39"/>
-      <c r="P71" s="40"/>
+      <c r="N71" s="44"/>
+      <c r="O71" s="44"/>
+      <c r="P71" s="45"/>
     </row>
     <row r="72" ht="15.75" customHeight="1">
       <c r="A72" s="3" t="s">
@@ -8723,13 +8744,13 @@
         <v>70.0</v>
       </c>
       <c r="C72" s="9"/>
-      <c r="M72" s="41">
+      <c r="M72" s="46">
         <v>185.0</v>
       </c>
-      <c r="N72" s="42">
+      <c r="N72" s="47">
         <v>62.0</v>
       </c>
-      <c r="O72" s="42">
+      <c r="O72" s="47">
         <v>128.0</v>
       </c>
       <c r="P72" s="13">
@@ -8744,15 +8765,15 @@
         <v>71.0</v>
       </c>
       <c r="C73" s="9"/>
-      <c r="M73" s="43" t="str">
+      <c r="M73" s="48" t="str">
         <f t="shared" ref="M73:P73" si="17">DEC2BIN(M72,8)</f>
         <v>10111001</v>
       </c>
-      <c r="N73" s="44" t="str">
+      <c r="N73" s="49" t="str">
         <f t="shared" si="17"/>
         <v>00111110</v>
       </c>
-      <c r="O73" s="44" t="str">
+      <c r="O73" s="49" t="str">
         <f t="shared" si="17"/>
         <v>10000000</v>
       </c>
@@ -8769,11 +8790,11 @@
         <v>72.0</v>
       </c>
       <c r="C74" s="9"/>
-      <c r="M74" s="38" t="s">
+      <c r="M74" s="43" t="s">
         <v>120</v>
       </c>
-      <c r="N74" s="39"/>
-      <c r="O74" s="39"/>
+      <c r="N74" s="44"/>
+      <c r="O74" s="44"/>
       <c r="P74" s="13" t="s">
         <v>3</v>
       </c>
@@ -8786,13 +8807,13 @@
         <v>73.0</v>
       </c>
       <c r="C75" s="9"/>
-      <c r="M75" s="41">
+      <c r="M75" s="46">
         <v>255.0</v>
       </c>
-      <c r="N75" s="42">
+      <c r="N75" s="47">
         <v>255.0</v>
       </c>
-      <c r="O75" s="42">
+      <c r="O75" s="47">
         <v>255.0</v>
       </c>
       <c r="P75" s="13">
@@ -8807,15 +8828,15 @@
         <v>74.0</v>
       </c>
       <c r="C76" s="9"/>
-      <c r="M76" s="43" t="str">
+      <c r="M76" s="48" t="str">
         <f t="shared" ref="M76:P76" si="18">DEC2BIN(M75,8)</f>
         <v>11111111</v>
       </c>
-      <c r="N76" s="44" t="str">
+      <c r="N76" s="49" t="str">
         <f t="shared" si="18"/>
         <v>11111111</v>
       </c>
-      <c r="O76" s="44" t="str">
+      <c r="O76" s="49" t="str">
         <f t="shared" si="18"/>
         <v>11111111</v>
       </c>

</xml_diff>

<commit_message>
elírt 30-as hálózatok javítása
</commit_message>
<xml_diff>
--- a/ipcim.xlsx
+++ b/ipcim.xlsx
@@ -325,10 +325,10 @@
     <t>O hálózat</t>
   </si>
   <si>
-    <t>10.0.0.3</t>
-  </si>
-  <si>
-    <t>10.0.0.4</t>
+    <t>10.0.0.5</t>
+  </si>
+  <si>
+    <t>10.0.0.6</t>
   </si>
   <si>
     <t>185.62.128.127</t>
@@ -343,22 +343,22 @@
     <t>185.62.128.223</t>
   </si>
   <si>
-    <t>10.0.0.5</t>
-  </si>
-  <si>
-    <t>10.0.0.6</t>
+    <t>10.0.0.9</t>
+  </si>
+  <si>
+    <t>10.0.0.10</t>
   </si>
   <si>
     <t>K hálózat</t>
   </si>
   <si>
-    <t>10.0.0.7</t>
+    <t>10.0.0.13</t>
   </si>
   <si>
     <t>R_BP</t>
   </si>
   <si>
-    <t>10.0.0.8</t>
+    <t>10.0.0.14</t>
   </si>
   <si>
     <t>Alhálózati cím</t>
@@ -661,7 +661,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="58">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -727,11 +727,20 @@
     <xf borderId="1" fillId="4" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
+    <xf borderId="1" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="1" fillId="5" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
+    <xf borderId="1" fillId="6" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="1" fillId="6" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="7" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
     <xf borderId="1" fillId="7" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
@@ -6410,10 +6419,10 @@
       <c r="Q7" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="R7" s="17" t="s">
+      <c r="R7" s="39" t="s">
         <v>102</v>
       </c>
-      <c r="S7" s="39" t="s">
+      <c r="S7" s="40" t="s">
         <v>97</v>
       </c>
     </row>
@@ -6455,10 +6464,10 @@
       <c r="Q8" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="R8" s="17" t="s">
+      <c r="R8" s="39" t="s">
         <v>103</v>
       </c>
-      <c r="S8" s="39" t="s">
+      <c r="S8" s="40" t="s">
         <v>97</v>
       </c>
     </row>
@@ -6587,10 +6596,10 @@
       <c r="Q11" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="R11" s="19" t="s">
+      <c r="R11" s="41" t="s">
         <v>108</v>
       </c>
-      <c r="S11" s="40" t="s">
+      <c r="S11" s="42" t="s">
         <v>97</v>
       </c>
     </row>
@@ -6625,10 +6634,10 @@
       <c r="Q12" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="R12" s="19" t="s">
+      <c r="R12" s="41" t="s">
         <v>109</v>
       </c>
-      <c r="S12" s="40" t="s">
+      <c r="S12" s="42" t="s">
         <v>97</v>
       </c>
     </row>
@@ -6730,10 +6739,10 @@
       <c r="Q15" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="R15" s="21" t="s">
+      <c r="R15" s="43" t="s">
         <v>111</v>
       </c>
-      <c r="S15" s="41" t="s">
+      <c r="S15" s="44" t="s">
         <v>97</v>
       </c>
     </row>
@@ -6768,10 +6777,10 @@
       <c r="Q16" s="21" t="s">
         <v>112</v>
       </c>
-      <c r="R16" s="21" t="s">
+      <c r="R16" s="43" t="s">
         <v>113</v>
       </c>
-      <c r="S16" s="41" t="s">
+      <c r="S16" s="44" t="s">
         <v>97</v>
       </c>
     </row>
@@ -6832,7 +6841,7 @@
       <c r="K18" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="M18" s="42" t="s">
+      <c r="M18" s="45" t="s">
         <v>87</v>
       </c>
       <c r="N18" s="31"/>
@@ -6865,12 +6874,12 @@
         <v>209.0</v>
       </c>
       <c r="K19" s="27"/>
-      <c r="M19" s="43" t="s">
+      <c r="M19" s="46" t="s">
         <v>114</v>
       </c>
-      <c r="N19" s="44"/>
-      <c r="O19" s="44"/>
-      <c r="P19" s="45"/>
+      <c r="N19" s="47"/>
+      <c r="O19" s="47"/>
+      <c r="P19" s="48"/>
     </row>
     <row r="20">
       <c r="A20" s="3" t="s">
@@ -6898,13 +6907,13 @@
         <v>210.0</v>
       </c>
       <c r="K20" s="27"/>
-      <c r="M20" s="46">
+      <c r="M20" s="49">
         <v>185.0</v>
       </c>
-      <c r="N20" s="47">
+      <c r="N20" s="50">
         <v>62.0</v>
       </c>
-      <c r="O20" s="47">
+      <c r="O20" s="50">
         <v>128.0</v>
       </c>
       <c r="P20" s="13">
@@ -6937,15 +6946,15 @@
         <v>211.0</v>
       </c>
       <c r="K21" s="27"/>
-      <c r="M21" s="48" t="str">
+      <c r="M21" s="51" t="str">
         <f t="shared" ref="M21:P21" si="1">DEC2BIN(M20,8)</f>
         <v>10111001</v>
       </c>
-      <c r="N21" s="49" t="str">
+      <c r="N21" s="52" t="str">
         <f t="shared" si="1"/>
         <v>00111110</v>
       </c>
-      <c r="O21" s="49" t="str">
+      <c r="O21" s="52" t="str">
         <f t="shared" si="1"/>
         <v>10000000</v>
       </c>
@@ -6953,7 +6962,7 @@
         <f t="shared" si="1"/>
         <v>00000000</v>
       </c>
-      <c r="R21" s="50" t="s">
+      <c r="R21" s="53" t="s">
         <v>115</v>
       </c>
       <c r="S21" s="32"/>
@@ -6984,17 +6993,17 @@
         <v>212.0</v>
       </c>
       <c r="K22" s="27"/>
-      <c r="M22" s="43" t="s">
+      <c r="M22" s="46" t="s">
         <v>116</v>
       </c>
-      <c r="N22" s="44"/>
-      <c r="O22" s="44"/>
-      <c r="P22" s="45"/>
-      <c r="R22" s="51">
+      <c r="N22" s="47"/>
+      <c r="O22" s="47"/>
+      <c r="P22" s="48"/>
+      <c r="R22" s="54">
         <f>(127+63+31+16)*51</f>
         <v>12087</v>
       </c>
-      <c r="S22" s="52">
+      <c r="S22" s="55">
         <f>R22*394</f>
         <v>4762278</v>
       </c>
@@ -7025,22 +7034,22 @@
         <v>213.0</v>
       </c>
       <c r="K23" s="27"/>
-      <c r="M23" s="46">
+      <c r="M23" s="49">
         <v>185.0</v>
       </c>
-      <c r="N23" s="47">
+      <c r="N23" s="50">
         <v>62.0</v>
       </c>
-      <c r="O23" s="47">
+      <c r="O23" s="50">
         <v>128.0</v>
       </c>
       <c r="P23" s="13">
         <v>1.0</v>
       </c>
-      <c r="S23" s="47"/>
-      <c r="T23" s="47"/>
-      <c r="U23" s="47"/>
-      <c r="V23" s="47"/>
+      <c r="S23" s="50"/>
+      <c r="T23" s="50"/>
+      <c r="U23" s="50"/>
+      <c r="V23" s="50"/>
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="3" t="s">
@@ -7068,15 +7077,15 @@
         <v>214.0</v>
       </c>
       <c r="K24" s="27"/>
-      <c r="M24" s="48" t="str">
+      <c r="M24" s="51" t="str">
         <f t="shared" ref="M24:P24" si="2">DEC2BIN(M23,8)</f>
         <v>10111001</v>
       </c>
-      <c r="N24" s="49" t="str">
+      <c r="N24" s="52" t="str">
         <f t="shared" si="2"/>
         <v>00111110</v>
       </c>
-      <c r="O24" s="49" t="str">
+      <c r="O24" s="52" t="str">
         <f t="shared" si="2"/>
         <v>10000000</v>
       </c>
@@ -7084,10 +7093,10 @@
         <f t="shared" si="2"/>
         <v>00000001</v>
       </c>
-      <c r="S24" s="47"/>
-      <c r="T24" s="47"/>
-      <c r="U24" s="47"/>
-      <c r="V24" s="47"/>
+      <c r="S24" s="50"/>
+      <c r="T24" s="50"/>
+      <c r="U24" s="50"/>
+      <c r="V24" s="50"/>
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="3" t="s">
@@ -7115,16 +7124,16 @@
         <v>215.0</v>
       </c>
       <c r="K25" s="27"/>
-      <c r="M25" s="43" t="s">
+      <c r="M25" s="46" t="s">
         <v>117</v>
       </c>
-      <c r="N25" s="44"/>
-      <c r="O25" s="44"/>
-      <c r="P25" s="45"/>
-      <c r="S25" s="47"/>
-      <c r="T25" s="47"/>
-      <c r="U25" s="47"/>
-      <c r="V25" s="47"/>
+      <c r="N25" s="47"/>
+      <c r="O25" s="47"/>
+      <c r="P25" s="48"/>
+      <c r="S25" s="50"/>
+      <c r="T25" s="50"/>
+      <c r="U25" s="50"/>
+      <c r="V25" s="50"/>
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="3" t="s">
@@ -7152,22 +7161,22 @@
         <v>216.0</v>
       </c>
       <c r="K26" s="27"/>
-      <c r="M26" s="46">
+      <c r="M26" s="49">
         <v>185.0</v>
       </c>
-      <c r="N26" s="47">
+      <c r="N26" s="50">
         <v>62.0</v>
       </c>
-      <c r="O26" s="47">
+      <c r="O26" s="50">
         <v>128.0</v>
       </c>
       <c r="P26" s="13">
         <v>2.0</v>
       </c>
-      <c r="S26" s="47"/>
-      <c r="T26" s="47"/>
-      <c r="U26" s="47"/>
-      <c r="V26" s="47"/>
+      <c r="S26" s="50"/>
+      <c r="T26" s="50"/>
+      <c r="U26" s="50"/>
+      <c r="V26" s="50"/>
     </row>
     <row r="27" ht="15.75" customHeight="1">
       <c r="A27" s="3" t="s">
@@ -7195,15 +7204,15 @@
         <v>217.0</v>
       </c>
       <c r="K27" s="27"/>
-      <c r="M27" s="48" t="str">
+      <c r="M27" s="51" t="str">
         <f t="shared" ref="M27:P27" si="3">DEC2BIN(M26,8)</f>
         <v>10111001</v>
       </c>
-      <c r="N27" s="49" t="str">
+      <c r="N27" s="52" t="str">
         <f t="shared" si="3"/>
         <v>00111110</v>
       </c>
-      <c r="O27" s="49" t="str">
+      <c r="O27" s="52" t="str">
         <f t="shared" si="3"/>
         <v>10000000</v>
       </c>
@@ -7211,10 +7220,10 @@
         <f t="shared" si="3"/>
         <v>00000010</v>
       </c>
-      <c r="S27" s="47"/>
-      <c r="T27" s="47"/>
-      <c r="U27" s="47"/>
-      <c r="V27" s="47"/>
+      <c r="S27" s="50"/>
+      <c r="T27" s="50"/>
+      <c r="U27" s="50"/>
+      <c r="V27" s="50"/>
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="A28" s="3" t="s">
@@ -7242,16 +7251,16 @@
         <v>218.0</v>
       </c>
       <c r="K28" s="27"/>
-      <c r="M28" s="43" t="s">
+      <c r="M28" s="46" t="s">
         <v>118</v>
       </c>
-      <c r="N28" s="44"/>
-      <c r="O28" s="44"/>
-      <c r="P28" s="45"/>
-      <c r="S28" s="47"/>
-      <c r="T28" s="47"/>
-      <c r="U28" s="47"/>
-      <c r="V28" s="47"/>
+      <c r="N28" s="47"/>
+      <c r="O28" s="47"/>
+      <c r="P28" s="48"/>
+      <c r="S28" s="50"/>
+      <c r="T28" s="50"/>
+      <c r="U28" s="50"/>
+      <c r="V28" s="50"/>
     </row>
     <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="3" t="s">
@@ -7279,22 +7288,22 @@
         <v>219.0</v>
       </c>
       <c r="K29" s="27"/>
-      <c r="M29" s="46">
+      <c r="M29" s="49">
         <v>185.0</v>
       </c>
-      <c r="N29" s="47">
+      <c r="N29" s="50">
         <v>62.0</v>
       </c>
-      <c r="O29" s="47">
+      <c r="O29" s="50">
         <v>128.0</v>
       </c>
       <c r="P29" s="13">
         <v>126.0</v>
       </c>
-      <c r="S29" s="47"/>
-      <c r="T29" s="47"/>
-      <c r="U29" s="47"/>
-      <c r="V29" s="47"/>
+      <c r="S29" s="50"/>
+      <c r="T29" s="50"/>
+      <c r="U29" s="50"/>
+      <c r="V29" s="50"/>
     </row>
     <row r="30" ht="15.75" customHeight="1">
       <c r="A30" s="3" t="s">
@@ -7322,15 +7331,15 @@
         <v>220.0</v>
       </c>
       <c r="K30" s="27"/>
-      <c r="M30" s="48" t="str">
+      <c r="M30" s="51" t="str">
         <f t="shared" ref="M30:P30" si="4">DEC2BIN(M29,8)</f>
         <v>10111001</v>
       </c>
-      <c r="N30" s="49" t="str">
+      <c r="N30" s="52" t="str">
         <f t="shared" si="4"/>
         <v>00111110</v>
       </c>
-      <c r="O30" s="49" t="str">
+      <c r="O30" s="52" t="str">
         <f t="shared" si="4"/>
         <v>10000000</v>
       </c>
@@ -7338,10 +7347,10 @@
         <f t="shared" si="4"/>
         <v>01111110</v>
       </c>
-      <c r="S30" s="47"/>
-      <c r="T30" s="47"/>
-      <c r="U30" s="47"/>
-      <c r="V30" s="47"/>
+      <c r="S30" s="50"/>
+      <c r="T30" s="50"/>
+      <c r="U30" s="50"/>
+      <c r="V30" s="50"/>
     </row>
     <row r="31" ht="15.75" customHeight="1">
       <c r="A31" s="3" t="s">
@@ -7369,17 +7378,17 @@
         <v>221.0</v>
       </c>
       <c r="K31" s="27"/>
-      <c r="M31" s="43" t="s">
+      <c r="M31" s="46" t="s">
         <v>119</v>
       </c>
-      <c r="N31" s="44"/>
-      <c r="O31" s="44"/>
-      <c r="P31" s="45"/>
-      <c r="R31" s="47"/>
-      <c r="S31" s="47"/>
-      <c r="T31" s="47"/>
-      <c r="U31" s="47"/>
-      <c r="V31" s="47"/>
+      <c r="N31" s="47"/>
+      <c r="O31" s="47"/>
+      <c r="P31" s="48"/>
+      <c r="R31" s="50"/>
+      <c r="S31" s="50"/>
+      <c r="T31" s="50"/>
+      <c r="U31" s="50"/>
+      <c r="V31" s="50"/>
     </row>
     <row r="32" ht="15.75" customHeight="1">
       <c r="A32" s="3" t="s">
@@ -7409,23 +7418,23 @@
       <c r="K32" s="27" t="s">
         <v>86</v>
       </c>
-      <c r="M32" s="46">
+      <c r="M32" s="49">
         <v>185.0</v>
       </c>
-      <c r="N32" s="47">
+      <c r="N32" s="50">
         <v>62.0</v>
       </c>
-      <c r="O32" s="47">
+      <c r="O32" s="50">
         <v>128.0</v>
       </c>
       <c r="P32" s="13">
         <v>127.0</v>
       </c>
-      <c r="R32" s="47"/>
-      <c r="S32" s="47"/>
-      <c r="T32" s="47"/>
-      <c r="U32" s="47"/>
-      <c r="V32" s="47"/>
+      <c r="R32" s="50"/>
+      <c r="S32" s="50"/>
+      <c r="T32" s="50"/>
+      <c r="U32" s="50"/>
+      <c r="V32" s="50"/>
     </row>
     <row r="33" ht="15.75" customHeight="1">
       <c r="A33" s="3" t="s">
@@ -7455,15 +7464,15 @@
       <c r="K33" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="M33" s="48" t="str">
+      <c r="M33" s="51" t="str">
         <f t="shared" ref="M33:P33" si="5">DEC2BIN(M32,8)</f>
         <v>10111001</v>
       </c>
-      <c r="N33" s="49" t="str">
+      <c r="N33" s="52" t="str">
         <f t="shared" si="5"/>
         <v>00111110</v>
       </c>
-      <c r="O33" s="49" t="str">
+      <c r="O33" s="52" t="str">
         <f t="shared" si="5"/>
         <v>10000000</v>
       </c>
@@ -7471,11 +7480,11 @@
         <f t="shared" si="5"/>
         <v>01111111</v>
       </c>
-      <c r="R33" s="47"/>
-      <c r="S33" s="47"/>
-      <c r="T33" s="47"/>
-      <c r="U33" s="47"/>
-      <c r="V33" s="47"/>
+      <c r="R33" s="50"/>
+      <c r="S33" s="50"/>
+      <c r="T33" s="50"/>
+      <c r="U33" s="50"/>
+      <c r="V33" s="50"/>
     </row>
     <row r="34" ht="15.75" customHeight="1">
       <c r="A34" s="3" t="s">
@@ -7494,19 +7503,19 @@
         <v>160.0</v>
       </c>
       <c r="G34" s="25"/>
-      <c r="M34" s="43" t="s">
+      <c r="M34" s="46" t="s">
         <v>120</v>
       </c>
-      <c r="N34" s="44"/>
-      <c r="O34" s="44"/>
+      <c r="N34" s="47"/>
+      <c r="O34" s="47"/>
       <c r="P34" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="R34" s="47"/>
-      <c r="S34" s="47"/>
-      <c r="T34" s="47"/>
-      <c r="U34" s="47"/>
-      <c r="V34" s="47"/>
+      <c r="R34" s="50"/>
+      <c r="S34" s="50"/>
+      <c r="T34" s="50"/>
+      <c r="U34" s="50"/>
+      <c r="V34" s="50"/>
     </row>
     <row r="35" ht="15.75" customHeight="1">
       <c r="A35" s="3" t="s">
@@ -7525,23 +7534,23 @@
         <v>161.0</v>
       </c>
       <c r="G35" s="25"/>
-      <c r="M35" s="46">
+      <c r="M35" s="49">
         <v>255.0</v>
       </c>
-      <c r="N35" s="47">
+      <c r="N35" s="50">
         <v>255.0</v>
       </c>
-      <c r="O35" s="47">
+      <c r="O35" s="50">
         <v>255.0</v>
       </c>
       <c r="P35" s="13">
         <v>128.0</v>
       </c>
-      <c r="R35" s="47"/>
-      <c r="S35" s="47"/>
-      <c r="T35" s="47"/>
-      <c r="U35" s="47"/>
-      <c r="V35" s="47"/>
+      <c r="R35" s="50"/>
+      <c r="S35" s="50"/>
+      <c r="T35" s="50"/>
+      <c r="U35" s="50"/>
+      <c r="V35" s="50"/>
     </row>
     <row r="36" ht="15.75" customHeight="1">
       <c r="A36" s="3" t="s">
@@ -7569,15 +7578,15 @@
       <c r="K36" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="M36" s="48" t="str">
+      <c r="M36" s="51" t="str">
         <f t="shared" ref="M36:P36" si="6">DEC2BIN(M35,8)</f>
         <v>11111111</v>
       </c>
-      <c r="N36" s="49" t="str">
+      <c r="N36" s="52" t="str">
         <f t="shared" si="6"/>
         <v>11111111</v>
       </c>
-      <c r="O36" s="49" t="str">
+      <c r="O36" s="52" t="str">
         <f t="shared" si="6"/>
         <v>11111111</v>
       </c>
@@ -7585,11 +7594,11 @@
         <f t="shared" si="6"/>
         <v>10000000</v>
       </c>
-      <c r="R36" s="47"/>
-      <c r="S36" s="47"/>
-      <c r="T36" s="47"/>
-      <c r="U36" s="47"/>
-      <c r="V36" s="47"/>
+      <c r="R36" s="50"/>
+      <c r="S36" s="50"/>
+      <c r="T36" s="50"/>
+      <c r="U36" s="50"/>
+      <c r="V36" s="50"/>
     </row>
     <row r="37" ht="15.75" customHeight="1">
       <c r="A37" s="3" t="s">
@@ -7617,14 +7626,14 @@
       <c r="K37" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="M37" s="47"/>
-      <c r="N37" s="47"/>
-      <c r="O37" s="47"/>
-      <c r="P37" s="47"/>
-      <c r="S37" s="47"/>
-      <c r="T37" s="47"/>
-      <c r="U37" s="47"/>
-      <c r="V37" s="47"/>
+      <c r="M37" s="50"/>
+      <c r="N37" s="50"/>
+      <c r="O37" s="50"/>
+      <c r="P37" s="50"/>
+      <c r="S37" s="50"/>
+      <c r="T37" s="50"/>
+      <c r="U37" s="50"/>
+      <c r="V37" s="50"/>
     </row>
     <row r="38" ht="15.75" customHeight="1">
       <c r="A38" s="3" t="s">
@@ -7652,16 +7661,16 @@
       <c r="K38" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="M38" s="53" t="s">
+      <c r="M38" s="56" t="s">
         <v>88</v>
       </c>
       <c r="N38" s="31"/>
       <c r="O38" s="31"/>
       <c r="P38" s="32"/>
-      <c r="S38" s="47"/>
-      <c r="T38" s="47"/>
-      <c r="U38" s="47"/>
-      <c r="V38" s="47"/>
+      <c r="S38" s="50"/>
+      <c r="T38" s="50"/>
+      <c r="U38" s="50"/>
+      <c r="V38" s="50"/>
     </row>
     <row r="39" ht="15.75" customHeight="1">
       <c r="A39" s="3" t="s">
@@ -7689,16 +7698,16 @@
       <c r="K39" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="M39" s="43" t="s">
+      <c r="M39" s="46" t="s">
         <v>114</v>
       </c>
-      <c r="N39" s="44"/>
-      <c r="O39" s="44"/>
-      <c r="P39" s="45"/>
-      <c r="S39" s="47"/>
-      <c r="T39" s="47"/>
-      <c r="U39" s="47"/>
-      <c r="V39" s="47"/>
+      <c r="N39" s="47"/>
+      <c r="O39" s="47"/>
+      <c r="P39" s="48"/>
+      <c r="S39" s="50"/>
+      <c r="T39" s="50"/>
+      <c r="U39" s="50"/>
+      <c r="V39" s="50"/>
     </row>
     <row r="40" ht="15.75" customHeight="1">
       <c r="A40" s="3" t="s">
@@ -7726,22 +7735,22 @@
       <c r="K40" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="M40" s="46">
+      <c r="M40" s="49">
         <v>185.0</v>
       </c>
-      <c r="N40" s="47">
+      <c r="N40" s="50">
         <v>62.0</v>
       </c>
-      <c r="O40" s="47">
+      <c r="O40" s="50">
         <v>128.0</v>
       </c>
       <c r="P40" s="13">
         <v>128.0</v>
       </c>
-      <c r="S40" s="47"/>
-      <c r="T40" s="47"/>
-      <c r="U40" s="47"/>
-      <c r="V40" s="47"/>
+      <c r="S40" s="50"/>
+      <c r="T40" s="50"/>
+      <c r="U40" s="50"/>
+      <c r="V40" s="50"/>
     </row>
     <row r="41" ht="15.75" customHeight="1">
       <c r="A41" s="3" t="s">
@@ -7769,15 +7778,15 @@
       <c r="K41" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="M41" s="48" t="str">
+      <c r="M41" s="51" t="str">
         <f t="shared" ref="M41:P41" si="7">DEC2BIN(M40,8)</f>
         <v>10111001</v>
       </c>
-      <c r="N41" s="49" t="str">
+      <c r="N41" s="52" t="str">
         <f t="shared" si="7"/>
         <v>00111110</v>
       </c>
-      <c r="O41" s="49" t="str">
+      <c r="O41" s="52" t="str">
         <f t="shared" si="7"/>
         <v>10000000</v>
       </c>
@@ -7785,10 +7794,10 @@
         <f t="shared" si="7"/>
         <v>10000000</v>
       </c>
-      <c r="S41" s="47"/>
-      <c r="T41" s="47"/>
-      <c r="U41" s="47"/>
-      <c r="V41" s="47"/>
+      <c r="S41" s="50"/>
+      <c r="T41" s="50"/>
+      <c r="U41" s="50"/>
+      <c r="V41" s="50"/>
     </row>
     <row r="42" ht="15.75" customHeight="1">
       <c r="A42" s="3" t="s">
@@ -7816,16 +7825,16 @@
       <c r="K42" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="M42" s="43" t="s">
+      <c r="M42" s="46" t="s">
         <v>116</v>
       </c>
-      <c r="N42" s="44"/>
-      <c r="O42" s="44"/>
-      <c r="P42" s="45"/>
-      <c r="S42" s="47"/>
-      <c r="T42" s="47"/>
-      <c r="U42" s="47"/>
-      <c r="V42" s="47"/>
+      <c r="N42" s="47"/>
+      <c r="O42" s="47"/>
+      <c r="P42" s="48"/>
+      <c r="S42" s="50"/>
+      <c r="T42" s="50"/>
+      <c r="U42" s="50"/>
+      <c r="V42" s="50"/>
     </row>
     <row r="43" ht="15.75" customHeight="1">
       <c r="A43" s="3" t="s">
@@ -7853,22 +7862,22 @@
       <c r="K43" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="M43" s="46">
+      <c r="M43" s="49">
         <v>185.0</v>
       </c>
-      <c r="N43" s="47">
+      <c r="N43" s="50">
         <v>62.0</v>
       </c>
-      <c r="O43" s="47">
+      <c r="O43" s="50">
         <v>128.0</v>
       </c>
       <c r="P43" s="13">
         <v>129.0</v>
       </c>
-      <c r="S43" s="47"/>
-      <c r="T43" s="47"/>
-      <c r="U43" s="47"/>
-      <c r="V43" s="47"/>
+      <c r="S43" s="50"/>
+      <c r="T43" s="50"/>
+      <c r="U43" s="50"/>
+      <c r="V43" s="50"/>
     </row>
     <row r="44" ht="15.75" customHeight="1">
       <c r="A44" s="3" t="s">
@@ -7896,15 +7905,15 @@
       <c r="K44" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="M44" s="48" t="str">
+      <c r="M44" s="51" t="str">
         <f t="shared" ref="M44:P44" si="8">DEC2BIN(M43,8)</f>
         <v>10111001</v>
       </c>
-      <c r="N44" s="49" t="str">
+      <c r="N44" s="52" t="str">
         <f t="shared" si="8"/>
         <v>00111110</v>
       </c>
-      <c r="O44" s="49" t="str">
+      <c r="O44" s="52" t="str">
         <f t="shared" si="8"/>
         <v>10000000</v>
       </c>
@@ -7912,10 +7921,10 @@
         <f t="shared" si="8"/>
         <v>10000001</v>
       </c>
-      <c r="S44" s="47"/>
-      <c r="T44" s="47"/>
-      <c r="U44" s="47"/>
-      <c r="V44" s="47"/>
+      <c r="S44" s="50"/>
+      <c r="T44" s="50"/>
+      <c r="U44" s="50"/>
+      <c r="V44" s="50"/>
     </row>
     <row r="45" ht="15.75" customHeight="1">
       <c r="A45" s="3" t="s">
@@ -7943,16 +7952,16 @@
       <c r="K45" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="M45" s="43" t="s">
+      <c r="M45" s="46" t="s">
         <v>117</v>
       </c>
-      <c r="N45" s="44"/>
-      <c r="O45" s="44"/>
-      <c r="P45" s="45"/>
-      <c r="S45" s="47"/>
-      <c r="T45" s="47"/>
-      <c r="U45" s="47"/>
-      <c r="V45" s="47"/>
+      <c r="N45" s="47"/>
+      <c r="O45" s="47"/>
+      <c r="P45" s="48"/>
+      <c r="S45" s="50"/>
+      <c r="T45" s="50"/>
+      <c r="U45" s="50"/>
+      <c r="V45" s="50"/>
     </row>
     <row r="46" ht="15.75" customHeight="1">
       <c r="A46" s="3" t="s">
@@ -7980,22 +7989,22 @@
       <c r="K46" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="M46" s="46">
+      <c r="M46" s="49">
         <v>185.0</v>
       </c>
-      <c r="N46" s="47">
+      <c r="N46" s="50">
         <v>62.0</v>
       </c>
-      <c r="O46" s="47">
+      <c r="O46" s="50">
         <v>128.0</v>
       </c>
       <c r="P46" s="13">
         <v>130.0</v>
       </c>
-      <c r="S46" s="47"/>
-      <c r="T46" s="47"/>
-      <c r="U46" s="47"/>
-      <c r="V46" s="47"/>
+      <c r="S46" s="50"/>
+      <c r="T46" s="50"/>
+      <c r="U46" s="50"/>
+      <c r="V46" s="50"/>
     </row>
     <row r="47" ht="15.75" customHeight="1">
       <c r="A47" s="3" t="s">
@@ -8023,15 +8032,15 @@
       <c r="K47" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="M47" s="48" t="str">
+      <c r="M47" s="51" t="str">
         <f t="shared" ref="M47:P47" si="9">DEC2BIN(M46,8)</f>
         <v>10111001</v>
       </c>
-      <c r="N47" s="49" t="str">
+      <c r="N47" s="52" t="str">
         <f t="shared" si="9"/>
         <v>00111110</v>
       </c>
-      <c r="O47" s="49" t="str">
+      <c r="O47" s="52" t="str">
         <f t="shared" si="9"/>
         <v>10000000</v>
       </c>
@@ -8039,10 +8048,10 @@
         <f t="shared" si="9"/>
         <v>10000010</v>
       </c>
-      <c r="S47" s="47"/>
-      <c r="T47" s="47"/>
-      <c r="U47" s="47"/>
-      <c r="V47" s="47"/>
+      <c r="S47" s="50"/>
+      <c r="T47" s="50"/>
+      <c r="U47" s="50"/>
+      <c r="V47" s="50"/>
     </row>
     <row r="48" ht="15.75" customHeight="1">
       <c r="A48" s="3" t="s">
@@ -8070,16 +8079,16 @@
       <c r="K48" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="M48" s="43" t="s">
+      <c r="M48" s="46" t="s">
         <v>118</v>
       </c>
-      <c r="N48" s="44"/>
-      <c r="O48" s="44"/>
-      <c r="P48" s="45"/>
-      <c r="S48" s="47"/>
-      <c r="T48" s="47"/>
-      <c r="U48" s="47"/>
-      <c r="V48" s="47"/>
+      <c r="N48" s="47"/>
+      <c r="O48" s="47"/>
+      <c r="P48" s="48"/>
+      <c r="S48" s="50"/>
+      <c r="T48" s="50"/>
+      <c r="U48" s="50"/>
+      <c r="V48" s="50"/>
     </row>
     <row r="49" ht="15.75" customHeight="1">
       <c r="A49" s="3" t="s">
@@ -8107,22 +8116,22 @@
       <c r="K49" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="M49" s="46">
+      <c r="M49" s="49">
         <v>185.0</v>
       </c>
-      <c r="N49" s="47">
+      <c r="N49" s="50">
         <v>62.0</v>
       </c>
-      <c r="O49" s="47">
+      <c r="O49" s="50">
         <v>128.0</v>
       </c>
       <c r="P49" s="13">
         <v>190.0</v>
       </c>
-      <c r="S49" s="47"/>
-      <c r="T49" s="47"/>
-      <c r="U49" s="47"/>
-      <c r="V49" s="47"/>
+      <c r="S49" s="50"/>
+      <c r="T49" s="50"/>
+      <c r="U49" s="50"/>
+      <c r="V49" s="50"/>
     </row>
     <row r="50" ht="15.75" customHeight="1">
       <c r="A50" s="3" t="s">
@@ -8150,15 +8159,15 @@
       <c r="K50" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="M50" s="48" t="str">
+      <c r="M50" s="51" t="str">
         <f t="shared" ref="M50:P50" si="10">DEC2BIN(M49,8)</f>
         <v>10111001</v>
       </c>
-      <c r="N50" s="49" t="str">
+      <c r="N50" s="52" t="str">
         <f t="shared" si="10"/>
         <v>00111110</v>
       </c>
-      <c r="O50" s="49" t="str">
+      <c r="O50" s="52" t="str">
         <f t="shared" si="10"/>
         <v>10000000</v>
       </c>
@@ -8166,10 +8175,10 @@
         <f t="shared" si="10"/>
         <v>10111110</v>
       </c>
-      <c r="S50" s="47"/>
-      <c r="T50" s="47"/>
-      <c r="U50" s="47"/>
-      <c r="V50" s="47"/>
+      <c r="S50" s="50"/>
+      <c r="T50" s="50"/>
+      <c r="U50" s="50"/>
+      <c r="V50" s="50"/>
     </row>
     <row r="51" ht="15.75" customHeight="1">
       <c r="A51" s="3" t="s">
@@ -8197,16 +8206,16 @@
       <c r="K51" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="M51" s="43" t="s">
+      <c r="M51" s="46" t="s">
         <v>119</v>
       </c>
-      <c r="N51" s="44"/>
-      <c r="O51" s="44"/>
-      <c r="P51" s="45"/>
-      <c r="S51" s="47"/>
-      <c r="T51" s="47"/>
-      <c r="U51" s="47"/>
-      <c r="V51" s="47"/>
+      <c r="N51" s="47"/>
+      <c r="O51" s="47"/>
+      <c r="P51" s="48"/>
+      <c r="S51" s="50"/>
+      <c r="T51" s="50"/>
+      <c r="U51" s="50"/>
+      <c r="V51" s="50"/>
     </row>
     <row r="52" ht="15.75" customHeight="1">
       <c r="A52" s="3" t="s">
@@ -8225,22 +8234,22 @@
         <v>178.0</v>
       </c>
       <c r="G52" s="25"/>
-      <c r="M52" s="46">
+      <c r="M52" s="49">
         <v>185.0</v>
       </c>
-      <c r="N52" s="47">
+      <c r="N52" s="50">
         <v>62.0</v>
       </c>
-      <c r="O52" s="47">
+      <c r="O52" s="50">
         <v>128.0</v>
       </c>
       <c r="P52" s="13">
         <v>191.0</v>
       </c>
-      <c r="S52" s="47"/>
-      <c r="T52" s="47"/>
-      <c r="U52" s="47"/>
-      <c r="V52" s="47"/>
+      <c r="S52" s="50"/>
+      <c r="T52" s="50"/>
+      <c r="U52" s="50"/>
+      <c r="V52" s="50"/>
     </row>
     <row r="53" ht="15.75" customHeight="1">
       <c r="A53" s="3" t="s">
@@ -8259,15 +8268,15 @@
         <v>179.0</v>
       </c>
       <c r="G53" s="25"/>
-      <c r="M53" s="48" t="str">
+      <c r="M53" s="51" t="str">
         <f t="shared" ref="M53:P53" si="11">DEC2BIN(M52,8)</f>
         <v>10111001</v>
       </c>
-      <c r="N53" s="49" t="str">
+      <c r="N53" s="52" t="str">
         <f t="shared" si="11"/>
         <v>00111110</v>
       </c>
-      <c r="O53" s="49" t="str">
+      <c r="O53" s="52" t="str">
         <f t="shared" si="11"/>
         <v>10000000</v>
       </c>
@@ -8293,11 +8302,11 @@
         <v>180.0</v>
       </c>
       <c r="G54" s="25"/>
-      <c r="M54" s="43" t="s">
+      <c r="M54" s="46" t="s">
         <v>120</v>
       </c>
-      <c r="N54" s="44"/>
-      <c r="O54" s="44"/>
+      <c r="N54" s="47"/>
+      <c r="O54" s="47"/>
       <c r="P54" s="13" t="s">
         <v>4</v>
       </c>
@@ -8319,13 +8328,13 @@
         <v>181.0</v>
       </c>
       <c r="G55" s="25"/>
-      <c r="M55" s="46">
+      <c r="M55" s="49">
         <v>255.0</v>
       </c>
-      <c r="N55" s="47">
+      <c r="N55" s="50">
         <v>255.0</v>
       </c>
-      <c r="O55" s="47">
+      <c r="O55" s="50">
         <v>255.0</v>
       </c>
       <c r="P55" s="13">
@@ -8349,15 +8358,15 @@
         <v>182.0</v>
       </c>
       <c r="G56" s="25"/>
-      <c r="M56" s="48" t="str">
+      <c r="M56" s="51" t="str">
         <f t="shared" ref="M56:P56" si="12">DEC2BIN(M55,8)</f>
         <v>11111111</v>
       </c>
-      <c r="N56" s="49" t="str">
+      <c r="N56" s="52" t="str">
         <f t="shared" si="12"/>
         <v>11111111</v>
       </c>
-      <c r="O56" s="49" t="str">
+      <c r="O56" s="52" t="str">
         <f t="shared" si="12"/>
         <v>11111111</v>
       </c>
@@ -8383,10 +8392,10 @@
         <v>183.0</v>
       </c>
       <c r="G57" s="25"/>
-      <c r="M57" s="47"/>
-      <c r="N57" s="47"/>
-      <c r="O57" s="47"/>
-      <c r="P57" s="47"/>
+      <c r="M57" s="50"/>
+      <c r="N57" s="50"/>
+      <c r="O57" s="50"/>
+      <c r="P57" s="50"/>
     </row>
     <row r="58" ht="15.75" customHeight="1">
       <c r="A58" s="3" t="s">
@@ -8405,7 +8414,7 @@
         <v>184.0</v>
       </c>
       <c r="G58" s="25"/>
-      <c r="M58" s="54" t="s">
+      <c r="M58" s="57" t="s">
         <v>89</v>
       </c>
       <c r="N58" s="31"/>
@@ -8429,12 +8438,12 @@
         <v>185.0</v>
       </c>
       <c r="G59" s="25"/>
-      <c r="M59" s="43" t="s">
+      <c r="M59" s="46" t="s">
         <v>114</v>
       </c>
-      <c r="N59" s="44"/>
-      <c r="O59" s="44"/>
-      <c r="P59" s="45"/>
+      <c r="N59" s="47"/>
+      <c r="O59" s="47"/>
+      <c r="P59" s="48"/>
     </row>
     <row r="60" ht="15.75" customHeight="1">
       <c r="A60" s="3" t="s">
@@ -8453,13 +8462,13 @@
         <v>186.0</v>
       </c>
       <c r="G60" s="25"/>
-      <c r="M60" s="46">
+      <c r="M60" s="49">
         <v>185.0</v>
       </c>
-      <c r="N60" s="47">
+      <c r="N60" s="50">
         <v>62.0</v>
       </c>
-      <c r="O60" s="47">
+      <c r="O60" s="50">
         <v>128.0</v>
       </c>
       <c r="P60" s="13">
@@ -8483,15 +8492,15 @@
         <v>187.0</v>
       </c>
       <c r="G61" s="25"/>
-      <c r="M61" s="48" t="str">
+      <c r="M61" s="51" t="str">
         <f t="shared" ref="M61:P61" si="13">DEC2BIN(M60,8)</f>
         <v>10111001</v>
       </c>
-      <c r="N61" s="49" t="str">
+      <c r="N61" s="52" t="str">
         <f t="shared" si="13"/>
         <v>00111110</v>
       </c>
-      <c r="O61" s="49" t="str">
+      <c r="O61" s="52" t="str">
         <f t="shared" si="13"/>
         <v>10000000</v>
       </c>
@@ -8517,12 +8526,12 @@
         <v>188.0</v>
       </c>
       <c r="G62" s="25"/>
-      <c r="M62" s="43" t="s">
+      <c r="M62" s="46" t="s">
         <v>116</v>
       </c>
-      <c r="N62" s="44"/>
-      <c r="O62" s="44"/>
-      <c r="P62" s="45"/>
+      <c r="N62" s="47"/>
+      <c r="O62" s="47"/>
+      <c r="P62" s="48"/>
     </row>
     <row r="63" ht="15.75" customHeight="1">
       <c r="A63" s="3" t="s">
@@ -8541,13 +8550,13 @@
         <v>189.0</v>
       </c>
       <c r="G63" s="25"/>
-      <c r="M63" s="46">
+      <c r="M63" s="49">
         <v>185.0</v>
       </c>
-      <c r="N63" s="47">
+      <c r="N63" s="50">
         <v>62.0</v>
       </c>
-      <c r="O63" s="47">
+      <c r="O63" s="50">
         <v>128.0</v>
       </c>
       <c r="P63" s="13">
@@ -8573,15 +8582,15 @@
       <c r="G64" s="25" t="s">
         <v>83</v>
       </c>
-      <c r="M64" s="48" t="str">
+      <c r="M64" s="51" t="str">
         <f t="shared" ref="M64:P64" si="14">DEC2BIN(M63,8)</f>
         <v>10111001</v>
       </c>
-      <c r="N64" s="49" t="str">
+      <c r="N64" s="52" t="str">
         <f t="shared" si="14"/>
         <v>00111110</v>
       </c>
-      <c r="O64" s="49" t="str">
+      <c r="O64" s="52" t="str">
         <f t="shared" si="14"/>
         <v>10000000</v>
       </c>
@@ -8607,12 +8616,12 @@
       <c r="G65" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="M65" s="43" t="s">
+      <c r="M65" s="46" t="s">
         <v>117</v>
       </c>
-      <c r="N65" s="44"/>
-      <c r="O65" s="44"/>
-      <c r="P65" s="45"/>
+      <c r="N65" s="47"/>
+      <c r="O65" s="47"/>
+      <c r="P65" s="48"/>
     </row>
     <row r="66" ht="15.75" customHeight="1">
       <c r="A66" s="3" t="s">
@@ -8622,13 +8631,13 @@
         <v>64.0</v>
       </c>
       <c r="C66" s="9"/>
-      <c r="M66" s="46">
+      <c r="M66" s="49">
         <v>185.0</v>
       </c>
-      <c r="N66" s="47">
+      <c r="N66" s="50">
         <v>62.0</v>
       </c>
-      <c r="O66" s="47">
+      <c r="O66" s="50">
         <v>128.0</v>
       </c>
       <c r="P66" s="13">
@@ -8643,15 +8652,15 @@
         <v>65.0</v>
       </c>
       <c r="C67" s="9"/>
-      <c r="M67" s="48" t="str">
+      <c r="M67" s="51" t="str">
         <f t="shared" ref="M67:P67" si="15">DEC2BIN(M66,8)</f>
         <v>10111001</v>
       </c>
-      <c r="N67" s="49" t="str">
+      <c r="N67" s="52" t="str">
         <f t="shared" si="15"/>
         <v>00111110</v>
       </c>
-      <c r="O67" s="49" t="str">
+      <c r="O67" s="52" t="str">
         <f t="shared" si="15"/>
         <v>10000000</v>
       </c>
@@ -8668,12 +8677,12 @@
         <v>66.0</v>
       </c>
       <c r="C68" s="9"/>
-      <c r="M68" s="43" t="s">
+      <c r="M68" s="46" t="s">
         <v>118</v>
       </c>
-      <c r="N68" s="44"/>
-      <c r="O68" s="44"/>
-      <c r="P68" s="45"/>
+      <c r="N68" s="47"/>
+      <c r="O68" s="47"/>
+      <c r="P68" s="48"/>
     </row>
     <row r="69" ht="15.75" customHeight="1">
       <c r="A69" s="3" t="s">
@@ -8683,13 +8692,13 @@
         <v>67.0</v>
       </c>
       <c r="C69" s="9"/>
-      <c r="M69" s="46">
+      <c r="M69" s="49">
         <v>185.0</v>
       </c>
-      <c r="N69" s="47">
+      <c r="N69" s="50">
         <v>62.0</v>
       </c>
-      <c r="O69" s="47">
+      <c r="O69" s="50">
         <v>128.0</v>
       </c>
       <c r="P69" s="13">
@@ -8704,15 +8713,15 @@
         <v>68.0</v>
       </c>
       <c r="C70" s="9"/>
-      <c r="M70" s="48" t="str">
+      <c r="M70" s="51" t="str">
         <f t="shared" ref="M70:P70" si="16">DEC2BIN(M69,8)</f>
         <v>10111001</v>
       </c>
-      <c r="N70" s="49" t="str">
+      <c r="N70" s="52" t="str">
         <f t="shared" si="16"/>
         <v>00111110</v>
       </c>
-      <c r="O70" s="49" t="str">
+      <c r="O70" s="52" t="str">
         <f t="shared" si="16"/>
         <v>10000000</v>
       </c>
@@ -8729,12 +8738,12 @@
         <v>69.0</v>
       </c>
       <c r="C71" s="9"/>
-      <c r="M71" s="43" t="s">
+      <c r="M71" s="46" t="s">
         <v>119</v>
       </c>
-      <c r="N71" s="44"/>
-      <c r="O71" s="44"/>
-      <c r="P71" s="45"/>
+      <c r="N71" s="47"/>
+      <c r="O71" s="47"/>
+      <c r="P71" s="48"/>
     </row>
     <row r="72" ht="15.75" customHeight="1">
       <c r="A72" s="3" t="s">
@@ -8744,13 +8753,13 @@
         <v>70.0</v>
       </c>
       <c r="C72" s="9"/>
-      <c r="M72" s="46">
+      <c r="M72" s="49">
         <v>185.0</v>
       </c>
-      <c r="N72" s="47">
+      <c r="N72" s="50">
         <v>62.0</v>
       </c>
-      <c r="O72" s="47">
+      <c r="O72" s="50">
         <v>128.0</v>
       </c>
       <c r="P72" s="13">
@@ -8765,15 +8774,15 @@
         <v>71.0</v>
       </c>
       <c r="C73" s="9"/>
-      <c r="M73" s="48" t="str">
+      <c r="M73" s="51" t="str">
         <f t="shared" ref="M73:P73" si="17">DEC2BIN(M72,8)</f>
         <v>10111001</v>
       </c>
-      <c r="N73" s="49" t="str">
+      <c r="N73" s="52" t="str">
         <f t="shared" si="17"/>
         <v>00111110</v>
       </c>
-      <c r="O73" s="49" t="str">
+      <c r="O73" s="52" t="str">
         <f t="shared" si="17"/>
         <v>10000000</v>
       </c>
@@ -8790,11 +8799,11 @@
         <v>72.0</v>
       </c>
       <c r="C74" s="9"/>
-      <c r="M74" s="43" t="s">
+      <c r="M74" s="46" t="s">
         <v>120</v>
       </c>
-      <c r="N74" s="44"/>
-      <c r="O74" s="44"/>
+      <c r="N74" s="47"/>
+      <c r="O74" s="47"/>
       <c r="P74" s="13" t="s">
         <v>3</v>
       </c>
@@ -8807,13 +8816,13 @@
         <v>73.0</v>
       </c>
       <c r="C75" s="9"/>
-      <c r="M75" s="46">
+      <c r="M75" s="49">
         <v>255.0</v>
       </c>
-      <c r="N75" s="47">
+      <c r="N75" s="50">
         <v>255.0</v>
       </c>
-      <c r="O75" s="47">
+      <c r="O75" s="50">
         <v>255.0</v>
       </c>
       <c r="P75" s="13">
@@ -8828,15 +8837,15 @@
         <v>74.0</v>
       </c>
       <c r="C76" s="9"/>
-      <c r="M76" s="48" t="str">
+      <c r="M76" s="51" t="str">
         <f t="shared" ref="M76:P76" si="18">DEC2BIN(M75,8)</f>
         <v>11111111</v>
       </c>
-      <c r="N76" s="49" t="str">
+      <c r="N76" s="52" t="str">
         <f t="shared" si="18"/>
         <v>11111111</v>
       </c>
-      <c r="O76" s="49" t="str">
+      <c r="O76" s="52" t="str">
         <f t="shared" si="18"/>
         <v>11111111</v>
       </c>

</xml_diff>